<commit_message>
Updated version of Test Plan spreadsheet
</commit_message>
<xml_diff>
--- a/Movie Theater Ticketing System Test Plan.xlsx
+++ b/Movie Theater Ticketing System Test Plan.xlsx
@@ -3,19 +3,38 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3214214-244E-4670-B251-C5A4AA193668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FD0B2DC-F298-47BC-ADC2-2D111378BF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
+    <sheet name="Movie Theater Ticketing System " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="155">
+  <si>
+    <t>Movie Theater Ticketing System Test Plan</t>
+  </si>
   <si>
     <t>TestCaseId</t>
   </si>
@@ -29,6 +48,9 @@
     <t>Description/Test Summary</t>
   </si>
   <si>
+    <t>Pre-requisites</t>
+  </si>
+  <si>
     <t>Test Steps</t>
   </si>
   <si>
@@ -44,49 +66,485 @@
     <t>Test Executed By</t>
   </si>
   <si>
-    <t>Pre-requisites</t>
-  </si>
-  <si>
-    <t>GoogleSearch_1</t>
-  </si>
-  <si>
-    <t>Search_Bar_Module</t>
+    <t>Authentication_0</t>
+  </si>
+  <si>
+    <t>User Registration</t>
   </si>
   <si>
     <t>P0</t>
   </si>
   <si>
-    <t>Verify that when a user writes a search term and presses enter, search results should be displayed</t>
-  </si>
-  <si>
-    <t>Browser is launched</t>
-  </si>
-  <si>
-    <t>1. Write the url - http://google.com in the browser's URL bar and press enter.
-2. Once google.com is launched, write the search term - "Apple" in the google search bar.
-3. Press enter.</t>
-  </si>
-  <si>
-    <t>Search results related to 'apple' should be displayed</t>
-  </si>
-  <si>
-    <t>Search results with 'apple' keyword are displayed</t>
+    <t>Test user registration functionality.</t>
+  </si>
+  <si>
+    <t>User is not registered in the system.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the registration page.
+2. Enter a valid username, password, and email.
+3. Click the register button.</t>
+  </si>
+  <si>
+    <t>User is successfully registered and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>Registration was successful and confirmation message was displayed.</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>TesterK</t>
-  </si>
-  <si>
-    <t>Movie Theater Ticketing System Test Plan</t>
+    <t>Robert Ashe</t>
+  </si>
+  <si>
+    <t>Authentication_1</t>
+  </si>
+  <si>
+    <t>User Authentication</t>
+  </si>
+  <si>
+    <t>Test user login functionality.</t>
+  </si>
+  <si>
+    <t>User account with valid credentials exists in the system.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the login page. 
+2. Enter a valid username. 
+3. Enter a valid password. 
+4 Click the login button.</t>
+  </si>
+  <si>
+    <t>User is successfully logged in and redirected to the main dashboard.</t>
+  </si>
+  <si>
+    <t>Login was successful and user was redirected to the main dashboard.</t>
+  </si>
+  <si>
+    <t>Authentication_2</t>
+  </si>
+  <si>
+    <t>Test user logout functionality.</t>
+  </si>
+  <si>
+    <t>User is logged in to the system.</t>
+  </si>
+  <si>
+    <t>1. Click the logout button.</t>
+  </si>
+  <si>
+    <t>User is successfully logged out and redirected to the login page.</t>
+  </si>
+  <si>
+    <t>User is logged out and redirected to the login page.</t>
+  </si>
+  <si>
+    <t>User_Functions_0</t>
+  </si>
+  <si>
+    <t>Ticket Purchase</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Test ticket purchasing for a specific movie and showtime.</t>
+  </si>
+  <si>
+    <t>User is logged in. Desired movie and showtime are available.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the movie listing page.
+2. Select a movie.
+3. Choose a showtime.
+4. Select a seat.
+5. Click on the purchase ticket button.</t>
+  </si>
+  <si>
+    <t>Ticket is successfully purchased and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>Puchase was successful and confirmation was displayed</t>
+  </si>
+  <si>
+    <t>User_Functions_1</t>
+  </si>
+  <si>
+    <t>All details of the selected movie are displayed correctly.</t>
+  </si>
+  <si>
+    <t>User_Functions_2</t>
+  </si>
+  <si>
+    <t>View Purchase History</t>
+  </si>
+  <si>
+    <t>Test viewing of user's purchase history.</t>
+  </si>
+  <si>
+    <t>User is logged in and has previous ticket purchases.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the user profile page.
+2. Click on the view purchase history button.</t>
+  </si>
+  <si>
+    <t>A list of previously purchased tickets is displayed.</t>
+  </si>
+  <si>
+    <t>List of previous purchases was displayed successfully.</t>
+  </si>
+  <si>
+    <t>Staff_Functions_0</t>
+  </si>
+  <si>
+    <t>Update Movie Listing</t>
+  </si>
+  <si>
+    <t>Test the ability of theater staff to manually update movie listings.</t>
+  </si>
+  <si>
+    <t>Theater staff is logged in. Desired movie is listed in the system.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the movie management page.
+2. Select a movie.
+3. Update movie details.
+4. Save changes.</t>
+  </si>
+  <si>
+    <t>Movie details are successfully updated and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>Movie listing is updated successfully and confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>Staff_Functions_1</t>
+  </si>
+  <si>
+    <t>Change Ticket Pricing</t>
+  </si>
+  <si>
+    <t>Test the ability of theater staff to change ticket pricing.</t>
+  </si>
+  <si>
+    <t>Theater staff is logged in.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the ticket management page.
+2. Select a ticket.
+3. Update ticket price.
+4. Save changes.</t>
+  </si>
+  <si>
+    <t>Ticket price is successfully updated and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>Ticket price was updated and confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>Administrator_Functions_0</t>
+  </si>
+  <si>
+    <t>Manage User Account</t>
+  </si>
+  <si>
+    <t>Test the ability of the administrator to delete a user account.</t>
+  </si>
+  <si>
+    <t>Administrator is logged in. Desired user account exists.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the user management page.
+2. Select a user.
+3. Click on the delete user button.</t>
+  </si>
+  <si>
+    <t>User account is successfully deleted and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>User account is deleted and confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>Administrator_Functions_1</t>
+  </si>
+  <si>
+    <t>Extract Business Data</t>
+  </si>
+  <si>
+    <t>Test the ability of the administrator to extract business data for a specific date range.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator is logged in. </t>
+  </si>
+  <si>
+    <t>1. Navigate to the business data extraction page.
+2. Select a date range.
+3. Click on the extract data button.</t>
+  </si>
+  <si>
+    <t>Business data for the specified range is displayed.</t>
+  </si>
+  <si>
+    <t>Business data is displayed.</t>
+  </si>
+  <si>
+    <t>Movie _Functions_0</t>
+  </si>
+  <si>
+    <t>Get Show Times</t>
+  </si>
+  <si>
+    <t>Matthew Press</t>
+  </si>
+  <si>
+    <t>Get Details</t>
+  </si>
+  <si>
+    <t>Ticket_Functions_0</t>
+  </si>
+  <si>
+    <t>Generate Ticket</t>
+  </si>
+  <si>
+    <t>Ticket_Functions_1</t>
+  </si>
+  <si>
+    <t>Cancel Ticket</t>
+  </si>
+  <si>
+    <t>The movie ID exists.</t>
+  </si>
+  <si>
+    <t>Test a valid movie ID for showtimes.</t>
+  </si>
+  <si>
+    <t>The list of date and times for movie showing is displayed.</t>
+  </si>
+  <si>
+    <t>List of showtimes is displayed.</t>
+  </si>
+  <si>
+    <t>Test a valid movie ID for details.</t>
+  </si>
+  <si>
+    <t>Test the ability to generate a ticket with valid inputs.</t>
+  </si>
+  <si>
+    <t>The user ID and movie ID exists.</t>
+  </si>
+  <si>
+    <t>Ticket details is displayed.</t>
+  </si>
+  <si>
+    <t>Ticket object with details is displayed.</t>
+  </si>
+  <si>
+    <t>The ticket is successfully cancelled and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>The ticket is cancelled and confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>Mohammed Almousawi</t>
+  </si>
+  <si>
+    <t>Card Number 16D</t>
+  </si>
+  <si>
+    <t>Payment Reject</t>
+  </si>
+  <si>
+    <t>1. Navigate to the movie details page. 
+2. Enter in the movie ID.
+3. Click on the showtimes button.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the ticket cancellation page.
+2. Enter the ticket ID.
+3. Click on the cancel button.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the ticket purchase page.
+2. Enter the user ID, movie ID, and the seat number.
+3. Click on the purchase button.</t>
+  </si>
+  <si>
+    <t>The card type is successfully matched the 4 fist digits.</t>
+  </si>
+  <si>
+    <t>The 16 digits successfully matched the digits and type.</t>
+  </si>
+  <si>
+    <t>The system will force the customer to enter only digits to verify the month and year.</t>
+  </si>
+  <si>
+    <t>The system will validate if the customer need to type 3 or 4 digits CVV.</t>
+  </si>
+  <si>
+    <t>The payment is successfully authorized and the system will redirect to the payment confirmation with order number.</t>
+  </si>
+  <si>
+    <t>The payment is not successfully authorized and the system will redirect to the payment error page.</t>
+  </si>
+  <si>
+    <t>Validate if customer has entered 2 digits months and 4 digits year for CC expiration date.</t>
+  </si>
+  <si>
+    <t>Check if the CC card matches type entered.</t>
+  </si>
+  <si>
+    <t>Check if all information entered is valid.</t>
+  </si>
+  <si>
+    <t>Reject if all information entered is not valid.</t>
+  </si>
+  <si>
+    <t>Validate CVV security has 3 or 4 digits depending on CC type.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the movie details page. 
+2. Click on a movie title.
+3. Click on the details button.</t>
+  </si>
+  <si>
+    <t>Movie details are displayed.</t>
+  </si>
+  <si>
+    <t>Payment_GW_Card_Type</t>
+  </si>
+  <si>
+    <t>Payment_GW_Card_Number</t>
+  </si>
+  <si>
+    <t>Payment_GW_Card_EXP_Date</t>
+  </si>
+  <si>
+    <t>Payment_GW_Card_CVV</t>
+  </si>
+  <si>
+    <t>Payment_GW_Success</t>
+  </si>
+  <si>
+    <t>Payment_GW_Reject</t>
+  </si>
+  <si>
+    <t>Card Type</t>
+  </si>
+  <si>
+    <t>Card Expire Date</t>
+  </si>
+  <si>
+    <t>Credit Card Security</t>
+  </si>
+  <si>
+    <t>Payment Success</t>
+  </si>
+  <si>
+    <t>Validate that customer has entered 16 digits for CC number.</t>
+  </si>
+  <si>
+    <t>Valid ticket ID exists.</t>
+  </si>
+  <si>
+    <t>Test the ability to cancel a ticket.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Payment GW.
+2. Choose card type from drop-down menu.
+3. Ensure that te system has automatically verified card type by checking visual indicator.</t>
+  </si>
+  <si>
+    <t>The card number box will show green mark for validition.</t>
+  </si>
+  <si>
+    <t>The box field will verify and show a green mark.</t>
+  </si>
+  <si>
+    <t>The confirmation page will appear with transaction ID.</t>
+  </si>
+  <si>
+    <t>The cancellation page will appear with transaction ID.</t>
+  </si>
+  <si>
+    <t>4 digits has to match type card.</t>
+  </si>
+  <si>
+    <t>The box contain 4 boxes each box contain 4 digits.</t>
+  </si>
+  <si>
+    <t>The box contain 2 boxes , 1st box month (2)digits , 2nd box (4) digits for the year.</t>
+  </si>
+  <si>
+    <t>The box will validate if the card need 3 or 4 digits CVV depend on CC type.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Payment GW.
+2. Enter the 16 digits CC number.
+3. Enter the CVV security code.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the ticket cancellation page.
+2. Enter all details.
+3. Click on the checkout button.</t>
+  </si>
+  <si>
+    <t>The Payment GW will verify all information been entered with bank merchant.</t>
+  </si>
+  <si>
+    <t>Unit_Test_0</t>
+  </si>
+  <si>
+    <t>No prerequisites required.</t>
+  </si>
+  <si>
+    <t>Test valid username format.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Payment GW.
+2. Enter the 16 digits CC number.
+3. System will verify the 16 digits.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Payment GW.
+2. Enter the 16 digits CC number.
+3. Enter the month and year of the card expiration.</t>
+  </si>
+  <si>
+    <t>1. Navigate to login page.
+2. Enter a valid username.
+3. Check visual indicator.</t>
+  </si>
+  <si>
+    <t>Unit_Test_1</t>
+  </si>
+  <si>
+    <t>Test invalid username format.</t>
+  </si>
+  <si>
+    <t>1. Navigate to login page.
+2. Enter an invalid username.
+3. Check visual indicator.</t>
+  </si>
+  <si>
+    <t>Visual indicator near username input field turns green, indicating a valid username.</t>
+  </si>
+  <si>
+    <t>Visual indicator near username input field turns red, indicating an invalid username.</t>
+  </si>
+  <si>
+    <t>Indicator turned green.</t>
+  </si>
+  <si>
+    <t>Indicator turned red.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +579,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="4">
@@ -170,19 +639,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -200,6 +681,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,247 +974,743 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="99" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
     <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.453125" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7265625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.54296875" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.81640625" customWidth="1"/>
     <col min="8" max="8" width="17.1796875" customWidth="1"/>
     <col min="9" max="9" width="9.26953125" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="58.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="58.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="58.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="58.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="58.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="70" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="47" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
+      <c r="C22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="35.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -971,16 +1952,9 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA57FBF7-1D76-4824-A501-AD08D0BB7C00}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1bb03773-d85b-495d-bef5-a6af3deffede"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c20fbfb4-75b0-4f86-bab5-69c1b2d353da"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>